<commit_message>
Service Reference + scrum
service reference toegevoegd + scrum aangepast
</commit_message>
<xml_diff>
--- a/Scrum_Deel2.xlsx
+++ b/Scrum_Deel2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13785" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="week4" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Wat heb ik gedaan?</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>SQL script hermaken, code conventions opstellen, Webservice maken</t>
+  </si>
+  <si>
+    <t>mockups bijgewerkt, github in orde gebracht</t>
+  </si>
+  <si>
+    <t>kon eerst niet inloggen bij github (ondertussen wel)</t>
+  </si>
+  <si>
+    <t>security tabellen implementeren</t>
+  </si>
+  <si>
+    <t>Wcf service gemaakt, logging geïmplementeerd</t>
+  </si>
+  <si>
+    <t>Login en registratie begonnen</t>
   </si>
 </sst>
 </file>
@@ -544,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -613,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -640,24 +655,36 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="4"/>
     </row>
   </sheetData>

</xml_diff>